<commit_message>
update code and cleaning data
</commit_message>
<xml_diff>
--- a/OpText.xlsx
+++ b/OpText.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHAMT16\Desktop\StoreMapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHAMT16\Desktop\study\streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CEEC45-833B-445F-8392-57098D501AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A6E038-4FEB-411C-8D0E-02E4EF36B966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6BFC1F5C-11BE-4C3F-AB85-90066D8FD168}"/>
   </bookViews>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="311">
   <si>
     <t>Optional text</t>
   </si>
@@ -146,9 +168,6 @@
     <t>dhd</t>
   </si>
   <si>
-    <t>Đức Hòa Đông</t>
-  </si>
-  <si>
     <t xml:space="preserve"> x </t>
   </si>
   <si>
@@ -194,9 +213,6 @@
     <t>Tru</t>
   </si>
   <si>
-    <t>Tru dien</t>
-  </si>
-  <si>
     <t>Gần Ngọc Mai</t>
   </si>
   <si>
@@ -362,9 +378,6 @@
     <t>Nga 3</t>
   </si>
   <si>
-    <t>Nga ba</t>
-  </si>
-  <si>
     <t>Ngã Ba</t>
   </si>
   <si>
@@ -389,15 +402,9 @@
     <t>ngã Tư</t>
   </si>
   <si>
-    <t>Nga tu</t>
-  </si>
-  <si>
     <t>.xã</t>
   </si>
   <si>
-    <t>Ql</t>
-  </si>
-  <si>
     <t>Ủy ban</t>
   </si>
   <si>
@@ -500,9 +507,6 @@
     <t>ĐHT</t>
   </si>
   <si>
-    <t>Đức Hòa Thượng</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tb, </t>
   </si>
   <si>
@@ -539,9 +543,6 @@
     <t>DD CỔNG</t>
   </si>
   <si>
-    <t>Nô Pộk</t>
-  </si>
-  <si>
     <t>Nô Bộc</t>
   </si>
   <si>
@@ -551,9 +552,6 @@
     <t>khu dân cư</t>
   </si>
   <si>
-    <t>KDC</t>
-  </si>
-  <si>
     <t>Khu dân cư</t>
   </si>
   <si>
@@ -975,6 +973,27 @@
   </si>
   <si>
     <t>Chung Cư</t>
+  </si>
+  <si>
+    <t>đức hòa đông</t>
+  </si>
+  <si>
+    <t>kdc</t>
+  </si>
+  <si>
+    <t>nga ba</t>
+  </si>
+  <si>
+    <t>nga tu</t>
+  </si>
+  <si>
+    <t>nô pộk</t>
+  </si>
+  <si>
+    <t>đức hòa thượng</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1332,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64058DCE-8460-47B0-8092-78EEAE7DF1EE}">
-  <dimension ref="A1:B261"/>
+  <dimension ref="A1:D521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="A262" sqref="A262"/>
+    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="C310" sqref="C310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1354,50 +1373,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1407,109 +1426,109 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -1524,20 +1543,20 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B35" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1545,12 +1564,12 @@
         <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1560,17 +1579,17 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1585,7 +1604,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1595,106 +1614,109 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>34</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>304</v>
+      </c>
+      <c r="D49" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B50" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
@@ -1704,17 +1726,17 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
@@ -1739,37 +1761,37 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
@@ -1779,12 +1801,12 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -1797,7 +1819,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -1807,17 +1829,17 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -1832,427 +1854,427 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B94" t="s">
-        <v>170</v>
+        <v>305</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B95" t="s">
-        <v>170</v>
+        <v>305</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B96" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97" t="s">
         <v>72</v>
-      </c>
-      <c r="B97" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B99" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B100" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B101" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B102" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B103" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B104" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B105" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B107" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B108" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B109" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B110" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B111" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B112" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B113" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B114" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B115" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B116" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B117" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B118" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B119" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B120" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B122" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B123" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B126" t="s">
-        <v>107</v>
+        <v>306</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B127" t="s">
-        <v>107</v>
+        <v>306</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B128" t="s">
-        <v>107</v>
+        <v>306</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B129" t="s">
-        <v>107</v>
+        <v>306</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B130" t="s">
-        <v>107</v>
+        <v>306</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B131" t="s">
-        <v>116</v>
+        <v>307</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B132" t="s">
-        <v>116</v>
+        <v>307</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B133" t="s">
-        <v>116</v>
+        <v>307</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B134" t="s">
-        <v>107</v>
+        <v>307</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B135" t="s">
-        <v>116</v>
+        <v>307</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B136" t="s">
-        <v>116</v>
+        <v>307</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B141" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B142" t="s">
-        <v>166</v>
+        <v>308</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B143" t="s">
-        <v>166</v>
+        <v>308</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B144" t="s">
-        <v>166</v>
+        <v>308</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -2262,10 +2284,10 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B150" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -2285,36 +2307,36 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B156" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B157" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
@@ -2324,12 +2346,12 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -2339,22 +2361,22 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -2364,22 +2386,22 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -2389,43 +2411,43 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B173" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B174" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B179" t="s">
         <v>2</v>
@@ -2433,7 +2455,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B180" t="s">
         <v>2</v>
@@ -2441,7 +2463,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B181" t="s">
         <v>2</v>
@@ -2449,7 +2471,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -2459,73 +2481,73 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B186" t="s">
-        <v>51</v>
+        <v>298</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B187" t="s">
-        <v>51</v>
+        <v>298</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B188" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B189" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
+        <v>36</v>
+      </c>
+      <c r="B190" t="s">
         <v>37</v>
-      </c>
-      <c r="B190" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B191" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B192" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B193" t="s">
         <v>24</v>
@@ -2533,10 +2555,10 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B194" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
@@ -2549,7 +2571,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B196" t="s">
         <v>24</v>
@@ -2557,76 +2579,76 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B197" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B198" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B199" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
@@ -2636,338 +2658,1957 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B213" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B214" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B215" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B218" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B219" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B220" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B221" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B222" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B223" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B224" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B225" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B226" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B227" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B228" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B229" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B230" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B231" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B232" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B233" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B234" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B235" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B236" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B237" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B238" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B239" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B240" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B250" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" t="str" cm="1">
+        <f t="array" ref="A262:A521" xml:space="preserve"> LOWER(A2:A261)</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" t="str">
+        <v xml:space="preserve"> cửa hàng bên trái</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" t="str">
+        <v xml:space="preserve"> đức huệ long an, huyện đức huệ, long an</v>
+      </c>
+      <c r="B264" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" t="str">
+        <v xml:space="preserve"> rẻ trái </v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" t="str">
+        <v xml:space="preserve"> vừa qua </v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A267" t="str">
+        <v xml:space="preserve"> x </v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A268" t="str">
+        <v>( cách ngã tư cái bông 1km)</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" t="str">
+        <v>( cửa hàng bên trái)</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A270" t="str">
+        <v>( cửa hàng bên trái)</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A271" t="str">
+        <v>(kc)</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272" t="str">
+        <v>,xã nhị long phú  huyện càng long tỉnh trà vinh, xã nhị long phú, huyện càng long, trà vinh</v>
+      </c>
+      <c r="B272" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273" t="str">
+        <v>.đối diện tthcs tân thiền b</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" t="str">
+        <v>.đối diện tthcs tân thiềng b</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A275" t="str">
+        <v>.xã</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A276" t="str">
+        <v>100m</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A277" t="str">
+        <v>200m</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A278" t="str">
+        <v>30m</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A279" t="str">
+        <v>500m</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A280" t="str">
+        <v>50m</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A281" t="str">
+        <v>50m</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A282" t="str">
+        <v>ap</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A283" t="str">
+        <v>ap</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A284" t="str">
+        <v>ấp</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A285" t="str">
+        <v>ấp</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286" t="str">
+        <v xml:space="preserve">ap </v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A287" t="str">
+        <v>bên phải</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A288" t="str">
+        <v>bx</v>
+      </c>
+      <c r="B288" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A289" t="str">
+        <v>bx</v>
+      </c>
+      <c r="B289" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A290" t="str">
+        <v>bx</v>
+      </c>
+      <c r="B290" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A291" t="str">
+        <v>cách</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A292" t="str">
+        <v>cách</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A293" t="str">
+        <v xml:space="preserve">cạnh </v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" t="str">
+        <v xml:space="preserve">cạnh </v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295" t="str">
+        <v>cầu 7 n</v>
+      </c>
+      <c r="B295" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296" t="str">
+        <v>cf</v>
+      </c>
+      <c r="B296" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297" t="str">
+        <v>chạy xuống đường</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298" t="str">
+        <v>cho  giông luôn</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A299" t="str">
+        <v>cho  giông luôn</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A300" t="str">
+        <v>cũ</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A301" t="str">
+        <v>d.</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A302" t="str">
+        <v>đ.</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A303" t="str">
+        <v>đ.</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A304" t="str">
+        <v xml:space="preserve">đ. </v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A305" t="str">
+        <v>đ/d</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A306" t="str">
+        <v>đ/diện</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A307" t="str">
+        <v>dd cổng</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A308" t="str">
+        <v>dd cổng</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A309" t="str">
+        <v>dhd</v>
+      </c>
+      <c r="B309" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A310" t="str">
+        <v>đht</v>
+      </c>
+      <c r="B310" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A311" t="str">
+        <v>đht</v>
+      </c>
+      <c r="B311" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A312" t="str">
+        <v>đối diện</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A313" t="str">
+        <v>đối diện</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A314" t="str">
+        <v>đối diện</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A315" t="str">
+        <v xml:space="preserve">đối dien </v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A316" t="str">
+        <v>dưới</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A317" t="str">
+        <v>dưới chân</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A318" t="str">
+        <v xml:space="preserve">dưới chân </v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A319" t="str">
+        <v>đương</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A320" t="str">
+        <v>đường</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A321" t="str">
+        <v>đường</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A322" t="str">
+        <v xml:space="preserve">đuong so </v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A323" t="str">
+        <v>đường vô</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A324" t="str">
+        <v>đường vô</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A325" t="str">
+        <v>f.</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A326" t="str">
+        <v>f.</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A327" t="str">
+        <v>gàn</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A328" t="str">
+        <v>gân</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A329" t="str">
+        <v>gần</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A330" t="str">
+        <v>gần</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A331" t="str">
+        <v>gần</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A332" t="str">
+        <v>gần</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A333" t="str">
+        <v>gần cổng chào thuộc về</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A334" t="str">
+        <v xml:space="preserve">gần đường quẹo vô nhà nghỉ phượng hồng, </v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A335" t="str">
+        <v>gần ngọc mai</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A336" t="str">
+        <v>gần ngọc mai</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A337" t="str">
+        <v>gần vòng xoay</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A338" t="str">
+        <v>gần vòng xoay</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A339" t="str">
+        <v>h.</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A340" t="str">
+        <v>h.</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A341" t="str">
+        <v xml:space="preserve">hẻm </v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A342" t="str">
+        <v xml:space="preserve">hẻm </v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A343" t="str">
+        <v>hl</v>
+      </c>
+      <c r="B343" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A344" t="str">
+        <v>hướng về</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A345" t="str">
+        <v>hướng về</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A346" t="str">
+        <v xml:space="preserve">hướng về </v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A347" t="str">
+        <v>huyện</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A348" t="str">
+        <v>huyện</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A349" t="str">
+        <v>kc</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A350" t="str">
+        <v>kc</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A351" t="str">
+        <v xml:space="preserve">kế </v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A352" t="str">
+        <v>khóm</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A353" t="str">
+        <v>khóm</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A354" t="str">
+        <v>khu dân cư</v>
+      </c>
+      <c r="B354" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A355" t="str">
+        <v>khu dân cư</v>
+      </c>
+      <c r="B355" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A356" t="str">
+        <v>khu phố</v>
+      </c>
+      <c r="B356" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" t="str">
+        <v>khu phố</v>
+      </c>
+      <c r="B357" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" t="str">
+        <v>khu phố</v>
+      </c>
+      <c r="B358" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A359" t="str">
+        <v>khu vực</v>
+      </c>
+      <c r="B359" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360" t="str">
+        <v>khu vực</v>
+      </c>
+      <c r="B360" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" t="str">
+        <v>khu vực</v>
+      </c>
+      <c r="B361" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A362" t="str">
+        <v>kp</v>
+      </c>
+      <c r="B362" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363" t="str">
+        <v>kp 1</v>
+      </c>
+      <c r="B363" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364" t="str">
+        <v>kp 1</v>
+      </c>
+      <c r="B364" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A365" t="str">
+        <v>kp 10</v>
+      </c>
+      <c r="B365" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A366" t="str">
+        <v>kp 10</v>
+      </c>
+      <c r="B366" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A367" t="str">
+        <v>kp 2</v>
+      </c>
+      <c r="B367" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A368" t="str">
+        <v>kp 2</v>
+      </c>
+      <c r="B368" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A369" t="str">
+        <v>kp 3</v>
+      </c>
+      <c r="B369" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A370" t="str">
+        <v>kp 3</v>
+      </c>
+      <c r="B370" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A371" t="str">
+        <v>kp 4</v>
+      </c>
+      <c r="B371" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A372" t="str">
+        <v>kp 4</v>
+      </c>
+      <c r="B372" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A373" t="str">
+        <v>kp 5</v>
+      </c>
+      <c r="B373" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A374" t="str">
+        <v>kp 5</v>
+      </c>
+      <c r="B374" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A375" t="str">
+        <v>kp 6</v>
+      </c>
+      <c r="B375" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A376" t="str">
+        <v>kp 6</v>
+      </c>
+      <c r="B376" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A377" t="str">
+        <v>kp 7</v>
+      </c>
+      <c r="B377" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A378" t="str">
+        <v>kp 7</v>
+      </c>
+      <c r="B378" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A379" t="str">
+        <v>kp 8</v>
+      </c>
+      <c r="B379" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A380" t="str">
+        <v>kp 8</v>
+      </c>
+      <c r="B380" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A381" t="str">
+        <v>kp 9</v>
+      </c>
+      <c r="B381" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A382" t="str">
+        <v>kp 9</v>
+      </c>
+      <c r="B382" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A383" t="str">
+        <v xml:space="preserve">lộ </v>
+      </c>
+      <c r="B383" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A384" t="str">
+        <v>lộ xã</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A385" t="str">
+        <v>lộ xã</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A386" t="str">
+        <v>nga 3</v>
+      </c>
+      <c r="B386" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A387" t="str">
+        <v>nga 3</v>
+      </c>
+      <c r="B387" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A388" t="str">
+        <v>ngã 3</v>
+      </c>
+      <c r="B388" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A389" t="str">
+        <v>ngã 3</v>
+      </c>
+      <c r="B389" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A390" t="str">
+        <v>ngã 3</v>
+      </c>
+      <c r="B390" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A391" t="str">
+        <v>nga 4</v>
+      </c>
+      <c r="B391" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A258" t="s">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A392" t="str">
+        <v>nga 4</v>
+      </c>
+      <c r="B392" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A393" t="str">
+        <v>ngã 4</v>
+      </c>
+      <c r="B393" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A394" t="str">
+        <v>ngã ba</v>
+      </c>
+      <c r="B394" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A395" t="str">
+        <v>ngã tư</v>
+      </c>
+      <c r="B395" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A396" t="str">
+        <v>ngã tư</v>
+      </c>
+      <c r="B396" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A397" t="str">
+        <v>ngã tư làng mới đường xuống</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A398" t="str">
+        <v>ngay</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A399" t="str">
+        <v>ngay</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A400" t="str">
+        <v>ngay</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A401" t="str">
+        <v>nhà nghỉ ng phương</v>
+      </c>
+      <c r="B401" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A402" t="str">
+        <v>nô bộc</v>
+      </c>
+      <c r="B402" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A259" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A260" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A261" t="s">
-        <v>311</v>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A403" t="str">
+        <v>nô bộc</v>
+      </c>
+      <c r="B403" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A404" t="str">
+        <v>nô bộc</v>
+      </c>
+      <c r="B404" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A405" t="str">
+        <v>phía sau tgdđ</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A406" t="str">
+        <v>phía sau tgdđ</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A407" t="str">
+        <v>phường</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A408" t="str">
+        <v>phường</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A409" t="str">
+        <v>qa</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A410" t="str">
+        <v>ql</v>
+      </c>
+      <c r="B410" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A411" t="str">
+        <v>qua</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A412" t="str">
+        <v>qua</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A413" t="str">
+        <v>qua khỏi</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A414" t="str">
+        <v>quẹo trái 100m</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A415" t="str">
+        <v xml:space="preserve">quốc lộ </v>
+      </c>
+      <c r="B415" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A416" t="str">
+        <v xml:space="preserve">quốc lộ </v>
+      </c>
+      <c r="B416" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A417" t="str">
+        <v xml:space="preserve">quốc lộ </v>
+      </c>
+      <c r="B417" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A418" t="str">
+        <v>quói an</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A419" t="str">
+        <v>quói an</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A420" t="str">
+        <v>rẽ phải 20m</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A421" t="str">
+        <v>rẽ phải vào 1km</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A422" t="str">
+        <v>sát</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A423" t="str">
+        <v>so</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A424" t="str">
+        <v>số</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A425" t="str">
+        <v>số</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A426" t="str">
+        <v>t1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A427" t="str">
+        <v>t1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A428" t="str">
+        <v xml:space="preserve">tb, </v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A429" t="str">
+        <v xml:space="preserve">tb, </v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A430" t="str">
+        <v xml:space="preserve">th </v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A431" t="str">
+        <v>thành phố</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A432" t="str">
+        <v>thành phố</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A433" t="str">
+        <v>thi tran</v>
+      </c>
+      <c r="B433" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A434" t="str">
+        <v>thị trấn</v>
+      </c>
+      <c r="B434" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A435" t="str">
+        <v>tiệm tôm</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A436" t="str">
+        <v>tiệm tôm</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A437" t="str">
+        <v>tỉnh</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A438" t="str">
+        <v>tỉnh</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A439" t="str">
+        <v>tỉnh lộ</v>
+      </c>
+      <c r="B439" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A440" t="str">
+        <v>tỉnh lộ</v>
+      </c>
+      <c r="B440" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A441" t="str">
+        <v xml:space="preserve">tl </v>
+      </c>
+      <c r="B441" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A442" t="str">
+        <v>tới</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A443" t="str">
+        <v>tp</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A444" t="str">
+        <v>trong</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A445" t="str">
+        <v>trong</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A446" t="str">
+        <v>tru</v>
+      </c>
+      <c r="B446" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A447" t="str">
+        <v>tru</v>
+      </c>
+      <c r="B447" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A448" t="str">
+        <v>tru dienng</v>
+      </c>
+      <c r="B448" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A449" t="str">
+        <v xml:space="preserve">tru dienong </v>
+      </c>
+      <c r="B449" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A450" t="str">
+        <v>tt</v>
+      </c>
+      <c r="B450" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A451" t="str">
+        <v>tt</v>
+      </c>
+      <c r="B451" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A452" t="str">
+        <v>tt.</v>
+      </c>
+      <c r="B452" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A453" t="str">
+        <v>ủb</v>
+      </c>
+      <c r="B453" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A454" t="str">
+        <v>ub chánh</v>
+      </c>
+      <c r="B454" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A455" t="str">
+        <v>ủy ban</v>
+      </c>
+      <c r="B455" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A456" t="str">
+        <v>ủy ban</v>
+      </c>
+      <c r="B456" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A457" t="str">
+        <v>ủy ban nhân dân</v>
+      </c>
+      <c r="B457" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A458" t="str">
+        <v>ủy ban nhân dân</v>
+      </c>
+      <c r="B458" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A459" t="str">
+        <v>ủy ban nhân dân</v>
+      </c>
+      <c r="B459" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A460" t="str">
+        <v>vào</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A461" t="str">
+        <v>vào</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A462" t="str">
+        <v>vào cổng</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A463" t="str">
+        <v>vào cổng</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A464" t="str">
+        <v>về</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A465" t="str">
+        <v>về</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A466" t="str">
+        <v>viet nam</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A467" t="str">
+        <v>việt nam</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A468" t="str">
+        <v>việt nam</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A469" t="str">
+        <v xml:space="preserve">vô </v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A470" t="str">
+        <v>x.</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A471" t="str">
+        <v>xã</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A472" t="str">
+        <v>xã</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A473" t="str">
+        <v>xa my hanh nam, xã mỹ hạnh nam</v>
+      </c>
+      <c r="B473" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A474" t="str">
+        <v xml:space="preserve">  ba tri bến tre  ba tri bến tre</v>
+      </c>
+      <c r="B474" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A475" t="str">
+        <v>ba tri bến tre ba tri bến tre</v>
+      </c>
+      <c r="B475" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A476" t="str">
+        <v>(</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A477" t="str">
+        <v>)</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A478" t="str">
+        <v>ba tri bến tre ba tri bến tre ba tri bến tre</v>
+      </c>
+      <c r="B478" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A479" t="str">
+        <v xml:space="preserve"> thị trấn bình đại bến tre thị trấn bình đại bình đại bến tre</v>
+      </c>
+      <c r="B479" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A480" t="str">
+        <v>bình đại bến tre bình đại bến tre</v>
+      </c>
+      <c r="B480" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A481" t="str">
+        <v>bến tre phú đức châu thành bến tre châu thành</v>
+      </c>
+      <c r="B481" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A482" t="str">
+        <v>chợ lách bến tre chợ lách bến tre</v>
+      </c>
+      <c r="B482" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A483" t="str">
+        <v>giồng trôm bến tre giồng trôm bến tre</v>
+      </c>
+      <c r="B483" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A484" t="str">
+        <v>mỏ cày bắc bến tre mỏ cày bắc bến tre</v>
+      </c>
+      <c r="B484" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A485" t="str">
+        <v>mỏ cày nam bến tre mỏ cày nam bến tre</v>
+      </c>
+      <c r="B485" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A486" t="str">
+        <v>thạnh phú bến tre thạnh phú bến tre</v>
+      </c>
+      <c r="B486" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A487" t="str">
+        <v>bến tre bến tre bến tre bến tre</v>
+      </c>
+      <c r="B487" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A488" t="str">
+        <v>đức hòa long an đức hòa long an</v>
+      </c>
+      <c r="B488" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A489" t="str">
+        <v>càng long trà vinh càng long trà vinh</v>
+      </c>
+      <c r="B489" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A490" t="str">
+        <v>bình phú càng long trà vinh bình phú càng long trà vinh càng long trà vinh</v>
+      </c>
+      <c r="B490" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A491" t="str">
+        <v>bình phú càng long trà vinh bình phú càng long trà vinh</v>
+      </c>
+      <c r="B491" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A492" t="str">
+        <v>cầu ngang trà vinh cầu ngang trà vinh</v>
+      </c>
+      <c r="B492" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A493" t="str">
+        <v>châu thành trà vinh châu thành trà vinh</v>
+      </c>
+      <c r="B493" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A494" t="str">
+        <v>công ty</v>
+      </c>
+      <c r="B494" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A495" t="str">
+        <v>ng lộc châu thành</v>
+      </c>
+      <c r="B495" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A496" t="str">
+        <v>thị duyên hải trà vinh thị duyên hải trà vinh</v>
+      </c>
+      <c r="B496" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A497" t="str">
+        <v>chợ cầu n thị trấn cầu n</v>
+      </c>
+      <c r="B497" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A498" t="str">
+        <v>tiểu cần trà vinh tiểu cần trà vinh</v>
+      </c>
+      <c r="B498" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A499" t="str">
+        <v>trà cú trà vinh trà cú trà vinh</v>
+      </c>
+      <c r="B499" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A500" t="str">
+        <v>nguyễn thị minh khai</v>
+      </c>
+      <c r="B500" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A501" t="str">
+        <v>tt. bình đại, bình đại, bến tre, việt nam,</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A502" t="str">
+        <v>chạy xuống</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A503" t="str">
+        <v>đường xuống</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A504" t="str">
+        <v>xuống</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A505" t="str">
+        <v xml:space="preserve">thị xã </v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A506" t="str">
+        <v>thị xã</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A507" t="str">
+        <v>tỉnh</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A508" t="str">
+        <v>tỉnh lộ</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A509" t="str">
+        <v>tp</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A510" t="str">
+        <v>f2</v>
+      </c>
+      <c r="B510" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A511" t="str">
+        <v>kp.</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A512" t="str">
+        <v>hẻm</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A513" t="str">
+        <v>c.đước</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A514" t="str">
+        <v>tru diện</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A515" t="str">
+        <v>tru điện</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A516" t="str">
+        <v>tru dien</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A517" t="str">
+        <v>kcn</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A518" t="str">
+        <v>ra</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A519" t="str">
+        <v>kd cư</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A520" t="str">
+        <v>khu chung cư</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A521" t="str">
+        <v>chung cư</v>
       </c>
     </row>
   </sheetData>

</xml_diff>